<commit_message>
changed tensile strain rate
</commit_message>
<xml_diff>
--- a/optimiser/input/__params__.xlsx
+++ b/optimiser/input/__params__.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/unsw/calibrate/optimiser/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBB00F81-F947-47CE-89AA-C89A0BBE51CB}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="225" windowWidth="28575" windowHeight="15375" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="3" r:id="rId1"/>
     <sheet name="evp" sheetId="5" r:id="rId2"/>
     <sheet name="evpcd" sheetId="6" r:id="rId3"/>
     <sheet name="evpwd" sheetId="7" r:id="rId4"/>
+    <sheet name="vshai" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="45">
   <si>
     <t>Temperature</t>
   </si>
@@ -145,6 +146,24 @@
   </si>
   <si>
     <t>C4,6,7,9</t>
+  </si>
+  <si>
+    <t>vsh_ts</t>
+  </si>
+  <si>
+    <t>vsh_b</t>
+  </si>
+  <si>
+    <t>vsh_t0</t>
+  </si>
+  <si>
+    <t>ai_g0</t>
+  </si>
+  <si>
+    <t>ai_n</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -292,6 +311,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,16 +586,16 @@
       <selection activeCell="B2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -593,24 +616,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEDA563-F318-4852-865D-A2318D089824}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
-    <col min="2" max="4" width="15.7109375" style="6" customWidth="1"/>
-    <col min="5" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="4"/>
-    <col min="11" max="13" width="9.140625" style="1"/>
-    <col min="14" max="15" width="9.140625" style="4"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.7265625" style="4" customWidth="1"/>
+    <col min="2" max="4" width="15.7265625" style="6" customWidth="1"/>
+    <col min="5" max="9" width="9.1796875" style="1"/>
+    <col min="10" max="10" width="9.1796875" style="4"/>
+    <col min="11" max="13" width="9.1796875" style="1"/>
+    <col min="14" max="15" width="9.1796875" style="4"/>
+    <col min="16" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -655,7 +678,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -690,7 +713,7 @@
         <v>1.0377930477444499E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -725,7 +748,7 @@
         <v>0.15624150805735959</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -763,7 +786,7 @@
         <v>2.226580145079296E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -798,116 +821,183 @@
         <v>7.3072064118940405E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="6">
         <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>800</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="1">
-        <v>67.982860006836731</v>
+        <v>265.97128364932661</v>
       </c>
       <c r="F7" s="1">
-        <v>99.076126653151491</v>
+        <v>2334.5423533249768</v>
       </c>
       <c r="G7" s="1">
-        <v>134.9013830759481</v>
+        <v>1.091355198813768</v>
       </c>
       <c r="H7" s="1">
-        <v>1.11085381164693</v>
+        <v>3.0705510178701112</v>
       </c>
       <c r="I7" s="1">
-        <v>39428.027905675168</v>
-      </c>
-      <c r="L7" s="8">
-        <v>2.448460628158876E-3</v>
+        <v>687.32156213341057</v>
+      </c>
+      <c r="L7" s="4">
+        <v>5.5741283847456228E-3</v>
       </c>
       <c r="M7" s="1">
-        <v>1.0303665491887431E-3</v>
-      </c>
-      <c r="N7" s="9">
-        <v>7.0566146733312802E-6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.1070907249626837E-5</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3.1070907249626837E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="6">
         <v>20</v>
-      </c>
-      <c r="B8" s="6">
-        <v>800</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="1">
+        <v>271.43761345714063</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1861.5090648936739</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.5523258274972089</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.2252593284146001</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5589.2001999798858</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1.1782549693226009E-2</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1.3882847727334001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6">
+        <v>800</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1">
+        <v>67.982860006836731</v>
+      </c>
+      <c r="F10" s="1">
+        <v>99.076126653151491</v>
+      </c>
+      <c r="G10" s="1">
+        <v>134.9013830759481</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.11085381164693</v>
+      </c>
+      <c r="I10" s="1">
+        <v>39428.027905675168</v>
+      </c>
+      <c r="L10" s="8">
+        <v>2.448460628158876E-3</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1.0303665491887431E-3</v>
+      </c>
+      <c r="N10" s="9">
+        <v>7.0566146733312802E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6">
+        <v>800</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1">
         <v>15.72914142100621</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F11" s="1">
         <v>98.979381984790848</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G11" s="1">
         <v>135.51557491245089</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H11" s="1">
         <v>12</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I11" s="1">
         <v>148.07714822857409</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L11" s="1">
         <v>2.4549495387739088E-3</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M11" s="1">
         <v>1.0160417592269E-3</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N11" s="4">
         <v>7.0591180944191226E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B12" s="6">
         <v>800</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E12" s="1">
         <v>3.3501042093951372</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F12" s="1">
         <v>98.861301913938064</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G12" s="1">
         <v>135.02815825225301</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H12" s="1">
         <v>20</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I12" s="1">
         <v>111.6171281516756</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L12" s="1">
         <v>2.4430788804578238E-3</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M12" s="1">
         <v>1.0403855337616061E-3</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N12" s="4">
         <v>7.0510364749994776E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L15" s="10"/>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="10"/>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="L18" s="10"/>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="G24" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -924,20 +1014,20 @@
       <selection activeCell="C31" sqref="A29:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="9.140625" style="4"/>
-    <col min="14" max="16" width="9.140625" style="1"/>
-    <col min="17" max="18" width="9.140625" style="4"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.7265625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="15.7265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="4"/>
+    <col min="6" max="12" width="9.1796875" style="1"/>
+    <col min="13" max="13" width="9.1796875" style="4"/>
+    <col min="14" max="16" width="9.1796875" style="1"/>
+    <col min="17" max="18" width="9.1796875" style="4"/>
+    <col min="19" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -991,7 +1081,7 @@
       </c>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -1042,7 +1132,7 @@
         <v>1.159485087826578E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -1092,7 +1182,7 @@
         <v>1.345243825392264E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1143,7 +1233,7 @@
         <v>1.4279890844544811E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1194,7 +1284,7 @@
         <v>1.48936285027564E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -1245,7 +1335,7 @@
         <v>1.5724421586219429E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1296,7 +1386,7 @@
         <v>1.595191044646898E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -1346,7 +1436,7 @@
         <v>1.7965440876793009E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
@@ -1396,7 +1486,7 @@
         <v>2.0595838947839451E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1536,7 @@
         <v>2.0775513706197801E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -1496,7 +1586,7 @@
         <v>2.082022164910018E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -1546,7 +1636,7 @@
         <v>1.8833986E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1596,7 +1686,7 @@
         <v>1.8911862000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
@@ -1649,7 +1739,7 @@
         <v>5.3435642999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1702,7 +1792,7 @@
         <v>5.3747182999999997E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -1752,7 +1842,7 @@
         <v>7.6125559999999995E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
@@ -1802,7 +1892,7 @@
         <v>7.6933159000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -1855,7 +1945,7 @@
         <v>0.14722453399999999</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -1908,7 +1998,7 @@
         <v>0.19619172000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -1961,7 +2051,7 @@
         <v>0.122089709</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -2024,23 +2114,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283AF620-1FFC-4E74-9A03-F7E60FF34CC2}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
-    <col min="2" max="4" width="15.7109375" style="6" customWidth="1"/>
-    <col min="5" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="9.140625" style="4"/>
-    <col min="14" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="9.140625" style="6"/>
-    <col min="18" max="18" width="9.140625" style="4"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.7265625" style="4" customWidth="1"/>
+    <col min="2" max="4" width="15.7265625" style="6" customWidth="1"/>
+    <col min="5" max="12" width="9.1796875" style="1"/>
+    <col min="13" max="13" width="9.1796875" style="4"/>
+    <col min="14" max="16" width="9.1796875" style="1"/>
+    <col min="17" max="17" width="9.1796875" style="6"/>
+    <col min="18" max="18" width="9.1796875" style="4"/>
+    <col min="19" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2184,7 @@
       </c>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -2144,7 +2234,7 @@
         <v>2.2841713E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2194,7 +2284,7 @@
         <v>2.4114355000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -2244,7 +2334,7 @@
         <v>2.5155472000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -2294,7 +2384,7 @@
         <v>2.8438244337302521E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -2344,7 +2434,7 @@
         <v>3.0089759010450551E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2394,7 +2484,7 @@
         <v>3.0959929041249609E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -2444,7 +2534,7 @@
         <v>3.4753224999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -2494,7 +2584,7 @@
         <v>3.4993432844805397E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -2544,7 +2634,7 @@
         <v>3.5595588999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -2594,7 +2684,7 @@
         <v>4.4154474999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -2644,7 +2734,7 @@
         <v>5.8251523999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -2694,7 +2784,7 @@
         <v>6.1723821999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -2747,7 +2837,7 @@
         <v>0.180131386</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
@@ -2800,7 +2890,7 @@
         <v>0.188443788</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -2853,7 +2943,7 @@
         <v>0.27976850599999997</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -2906,7 +2996,7 @@
         <v>0.28514160199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -2956,7 +3046,7 @@
         <v>0.119812076</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -3006,7 +3096,7 @@
         <v>0.12215622299999999</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -3059,7 +3149,7 @@
         <v>9.7729160999999995E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3119,4 +3209,104 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C31987-20C0-4713-874C-028D8E4E8744}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.7265625" style="4" customWidth="1"/>
+    <col min="2" max="4" width="15.7265625" style="6" customWidth="1"/>
+    <col min="5" max="9" width="9.1796875" style="1"/>
+    <col min="10" max="11" width="9.1796875" style="6"/>
+    <col min="12" max="12" width="9.1796875" style="4"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
+        <v>327.86500000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.60553000000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>81.307000000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>15</v>
+      </c>
+      <c r="J2" s="6">
+        <v>2.1678500999999999E-2</v>
+      </c>
+      <c r="K2" s="6">
+        <v>4.6995700000000001E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>